<commit_message>
Added report, updated code
</commit_message>
<xml_diff>
--- a/measurements/13122014.xlsx
+++ b/measurements/13122014.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Niek\Sync\Projects\WTherm-v2\measurements\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Niek\Sync\Projects\WTherm\measurements\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8145" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8145"/>
   </bookViews>
   <sheets>
     <sheet name="13122014" sheetId="1" r:id="rId1"/>
@@ -26,9 +26,6 @@
   </si>
   <si>
     <t>meter value (MJ)</t>
-  </si>
-  <si>
-    <t>Qin(MJ)</t>
   </si>
   <si>
     <t>Average dT</t>
@@ -52,9 +49,6 @@
     <t>KW</t>
   </si>
   <si>
-    <t xml:space="preserve">U = </t>
-  </si>
-  <si>
     <t>W/K</t>
   </si>
   <si>
@@ -71,9 +65,6 @@
   </si>
   <si>
     <t>°C</t>
-  </si>
-  <si>
-    <t>Qout (MJ)</t>
   </si>
   <si>
     <t>Heating up (06:00-12:00)</t>
@@ -106,17 +97,122 @@
     <t>Net heat</t>
   </si>
   <si>
-    <t>Qnet (MJ)</t>
+    <t>-</t>
   </si>
   <si>
-    <t>-</t>
+    <r>
+      <t>C</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>t</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Q</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>loss</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (MJ)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Q</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>net</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (MJ)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Q</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>in</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(MJ)</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -255,6 +351,14 @@
       <b/>
       <i/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -728,24 +832,24 @@
     <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
     <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
     <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Berekening" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Controlecel" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Gekoppelde cel" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Goed" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Invoer" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Kop 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Kop 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Kop 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Kop 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Neutraal" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Notitie" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Ongeldig" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
-    <cellStyle name="Titel" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Totaal" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Uitvoer" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Verklarende tekst" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Waarschuwingstekst" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -763,7 +867,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="nl-NL"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -800,7 +904,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -826,7 +929,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="nl-NL"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3110,8 +3213,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="209418616"/>
-        <c:axId val="209419792"/>
+        <c:axId val="-1125575680"/>
+        <c:axId val="-1125578400"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -4258,11 +4361,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="209424496"/>
-        <c:axId val="209422144"/>
+        <c:axId val="-1125573504"/>
+        <c:axId val="-1125569152"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="209418616"/>
+        <c:axId val="-1125575680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4302,10 +4405,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="209419792"/>
+        <c:crossAx val="-1125578400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4314,7 +4417,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="209419792"/>
+        <c:axId val="-1125578400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4367,7 +4470,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4393,7 +4495,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="nl-NL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -4425,15 +4527,15 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="209418616"/>
+        <c:crossAx val="-1125575680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="209422144"/>
+        <c:axId val="-1125569152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4465,7 +4567,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4491,7 +4592,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="nl-NL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -4523,15 +4624,15 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="209424496"/>
+        <c:crossAx val="-1125573504"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="209424496"/>
+        <c:axId val="-1125573504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4541,7 +4642,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="209422144"/>
+        <c:crossAx val="-1125569152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4558,7 +4659,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4584,7 +4684,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="nl-NL"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -4614,7 +4714,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="nl-NL"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -4628,7 +4728,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="nl-NL"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -4675,7 +4775,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4701,7 +4800,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="nl-NL"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -5833,8 +5932,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="209420184"/>
-        <c:axId val="209418224"/>
+        <c:axId val="-1125572416"/>
+        <c:axId val="-1125571328"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -6706,11 +6805,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="209423320"/>
-        <c:axId val="209419008"/>
+        <c:axId val="-1125571872"/>
+        <c:axId val="-1125570784"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="209420184"/>
+        <c:axId val="-1125572416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6750,10 +6849,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="209418224"/>
+        <c:crossAx val="-1125571328"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6762,7 +6861,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="209418224"/>
+        <c:axId val="-1125571328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6810,15 +6909,15 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="209420184"/>
+        <c:crossAx val="-1125572416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="209419008"/>
+        <c:axId val="-1125570784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6852,15 +6951,15 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="209423320"/>
+        <c:crossAx val="-1125571872"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="209423320"/>
+        <c:axId val="-1125571872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6870,7 +6969,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="209419008"/>
+        <c:crossAx val="-1125570784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6887,7 +6986,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6913,7 +7011,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="nl-NL"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -6943,7 +7041,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="nl-NL"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -6957,7 +7055,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="nl-NL"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -6999,7 +7097,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7025,7 +7122,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="nl-NL"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -8013,8 +8110,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="209423712"/>
-        <c:axId val="209417048"/>
+        <c:axId val="-1125564800"/>
+        <c:axId val="-1125568064"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -9505,11 +9602,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="209422928"/>
-        <c:axId val="209419400"/>
+        <c:axId val="-1125569696"/>
+        <c:axId val="-1125570240"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="209423712"/>
+        <c:axId val="-1125564800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9549,10 +9646,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="209417048"/>
+        <c:crossAx val="-1125568064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9561,7 +9658,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="209417048"/>
+        <c:axId val="-1125568064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="20"/>
@@ -9614,7 +9711,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -9640,7 +9736,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="nl-NL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -9672,15 +9768,15 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="209423712"/>
+        <c:crossAx val="-1125564800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="209419400"/>
+        <c:axId val="-1125570240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9717,7 +9813,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -9743,7 +9838,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="nl-NL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -9775,15 +9870,15 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="209422928"/>
+        <c:crossAx val="-1125569696"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="209422928"/>
+        <c:axId val="-1125569696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9793,7 +9888,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="209419400"/>
+        <c:crossAx val="-1125570240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9810,7 +9905,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9836,7 +9930,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="nl-NL"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -9866,7 +9960,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="nl-NL"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -11647,9 +11741,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Kantoor">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -11687,7 +11781,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Kantoor">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -11759,7 +11853,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Kantoor">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -11911,8 +12005,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M866"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R23" sqref="R23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11935,19 +12029,19 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="G1" s="2" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>28</v>
@@ -11983,7 +12077,7 @@
         <v>-1.4511825390413429</v>
       </c>
       <c r="K2" s="14" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="L2" s="5"/>
       <c r="M2" s="6"/>
@@ -12051,14 +12145,14 @@
         <v>1.6464523835517308</v>
       </c>
       <c r="K4" s="15" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L4" s="8">
         <f>AVERAGE(D80:D164)-AVERAGE(E80:E164)</f>
         <v>14.292941176470583</v>
       </c>
       <c r="M4" s="16" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -12091,14 +12185,14 @@
         <v>1.1892323426573128</v>
       </c>
       <c r="K5" s="15" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L5" s="8">
         <f>(B164-B80)/3.6</f>
         <v>36.388888888888886</v>
       </c>
       <c r="M5" s="16" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -12131,14 +12225,14 @@
         <v>1.7271386580675658</v>
       </c>
       <c r="K6" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L6" s="10">
         <f>A164-A80</f>
         <v>0.29166666666424135</v>
       </c>
       <c r="M6" s="16" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -12171,14 +12265,14 @@
         <v>2.2492238103494628</v>
       </c>
       <c r="K7" s="15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L7" s="11">
         <f>L5/(L6*24)</f>
         <v>5.1984126984559245</v>
       </c>
       <c r="M7" s="16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -12211,14 +12305,14 @@
         <v>2.7920037694550448</v>
       </c>
       <c r="K8" s="15" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="L8" s="8">
         <f>1000*L7/L4</f>
         <v>363.70489700284281</v>
       </c>
       <c r="M8" s="16" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -12284,7 +12378,7 @@
         <v>3.8520316014797267</v>
       </c>
       <c r="K10" s="17" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="L10" s="8"/>
       <c r="M10" s="9"/>
@@ -12352,14 +12446,14 @@
         <v>4.9060219364426203</v>
       </c>
       <c r="K12" s="15" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="L12" s="8">
         <f>C74</f>
         <v>155</v>
       </c>
       <c r="M12" s="16" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -12392,14 +12486,14 @@
         <v>5.4221059580530273</v>
       </c>
       <c r="K13" s="15" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="L13" s="11">
         <f>(A74-A2)*24</f>
         <v>6</v>
       </c>
       <c r="M13" s="16" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -12432,14 +12526,14 @@
         <v>5.9381899775904259</v>
       </c>
       <c r="K14" s="15" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="L14" s="8">
         <f>(L12*1000000)/(L13*3600)/1000</f>
         <v>7.1759259259259265</v>
       </c>
       <c r="M14" s="16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -12505,14 +12599,14 @@
         <v>7.9535548526080753</v>
       </c>
       <c r="K16" s="15" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="L16" s="8">
         <f>H74</f>
         <v>36.8100202239727</v>
       </c>
       <c r="M16" s="16" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
@@ -12545,14 +12639,14 @@
         <v>8.4209024158034751</v>
       </c>
       <c r="K17" s="15" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="L17" s="8">
         <f>D74-D2</f>
         <v>4.0999999999999979</v>
       </c>
       <c r="M17" s="16" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
@@ -12585,14 +12679,14 @@
         <v>9.8824307029142631</v>
       </c>
       <c r="K18" s="15" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="L18" s="8">
         <f>(L16*10^6)/L17</f>
         <v>8978053.7131640781</v>
       </c>
       <c r="M18" s="16" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12625,7 +12719,7 @@
         <v>10.333047838796201</v>
       </c>
       <c r="K19" s="18" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="L19" s="12">
         <f>AVERAGE(E2:E74)</f>
@@ -19042,7 +19136,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="E18"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E13" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="E13" workbookViewId="0">
       <selection activeCell="V16" sqref="V16"/>
     </sheetView>
   </sheetViews>
@@ -19050,7 +19144,7 @@
   <sheetData>
     <row r="18" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E18" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>